<commit_message>
Fixed NPE in DeploymentProfile
NPE occurred when unknown variable was referenced in an interpolated
string.
</commit_message>
<xml_diff>
--- a/docs/pdtoolgui_bug_list.xlsx
+++ b/docs/pdtoolgui_bug_list.xlsx
@@ -10,7 +10,7 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$E$1:$I$85</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$E$1:$I$84</definedName>
   </definedNames>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="660" uniqueCount="167">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="653" uniqueCount="166">
   <si>
     <t>Reported By</t>
   </si>
@@ -368,10 +368,6 @@
     <t>buttonset refreshes not refreshing the correct ID's</t>
   </si>
   <si>
-    <t>Need to ship with default set of server attributes for 6.2. When user changes default server, GUI should regenerate attributes based on new default server.
-Need key event listener to update typeahead list as / chars are entered.</t>
-  </si>
-  <si>
     <t>Mike T is adding feature to let useHttps override encrypt in PDTool. Lowering priority.</t>
   </si>
   <si>
@@ -509,9 +505,6 @@
     <t>Server editor panel should have "test connection" button</t>
   </si>
   <si>
-    <t>Need to call Admin API SOAP service such as getLicenses</t>
-  </si>
-  <si>
     <t>VCS module generator needs to have vcs connection entry in target module XML file</t>
   </si>
   <si>
@@ -527,18 +520,12 @@
     <t>b2</t>
   </si>
   <si>
-    <t>Plan editor ID lookup needs to interpolate variables in module path by applying default profile variable values.</t>
-  </si>
-  <si>
     <t>Data source module generator writes map type attributes without empty valuemap tag. Causes PDTool to throw error claiming the data source does not have a name.</t>
   </si>
   <si>
     <t>Plan editor duplicates first row into new second row after dialog for second row is closed.</t>
   </si>
   <si>
-    <t>Need to roll in May 28 enhancements to PDTool.</t>
-  </si>
-  <si>
     <t>Plan editor check to see if module file has entries doesn't check to see if entry list is null</t>
   </si>
   <si>
@@ -548,7 +535,18 @@
     <t>Rowid generator returned NaN if plan list had no entries.</t>
   </si>
   <si>
-    <t>Need to modify generic attribute serializer to include empty valueMap tag. (Tentatively fixed, need to test with a deployment.)</t>
+    <t>Needed to modify generic attribute serializer to include empty valueMap tag.</t>
+  </si>
+  <si>
+    <t>Need to call Admin API SOAP service such as getLicenses from GUI server.</t>
+  </si>
+  <si>
+    <t>Need to ship with default set of server attributes for 6.2. When user changes default server, GUI should regenerate attributes based on new default server.
+Need key event listener to update typeahead list as / chars are entered.
+Need tree-based chooser dialog</t>
+  </si>
+  <si>
+    <t>NPE thrown when plan editor attempts to interpolate unset variable in module path</t>
   </si>
 </sst>
 </file>
@@ -605,8 +603,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="19">
+  <cellStyleXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -649,7 +649,7 @@
     </xf>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="19">
+  <cellStyles count="21">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -659,6 +659,7 @@
     <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="20" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -668,6 +669,7 @@
     <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="19" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -998,11 +1000,11 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr filterMode="1" enableFormatConditionsCalculation="0"/>
-  <dimension ref="A1:M85"/>
+  <dimension ref="A1:M84"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A66" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="M83" sqref="M83"/>
+      <pane ySplit="1" topLeftCell="A40" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A85" sqref="A85"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1110,7 +1112,7 @@
         <v>20</v>
       </c>
       <c r="G3" s="3" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="H3" s="3" t="s">
         <v>18</v>
@@ -1142,7 +1144,7 @@
         <v>20</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="H4" s="3" t="s">
         <v>18</v>
@@ -1177,7 +1179,7 @@
         <v>20</v>
       </c>
       <c r="G5" s="3" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="H5" s="3" t="s">
         <v>18</v>
@@ -1222,7 +1224,7 @@
         <v>58</v>
       </c>
       <c r="M6" s="4" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="7" spans="1:13">
@@ -1277,7 +1279,7 @@
         <v>20</v>
       </c>
       <c r="G8" s="3" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="H8" s="3" t="s">
         <v>17</v>
@@ -1318,7 +1320,7 @@
         <v>20</v>
       </c>
       <c r="G9" s="3" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="H9" s="3" t="s">
         <v>18</v>
@@ -1356,7 +1358,7 @@
         <v>20</v>
       </c>
       <c r="G10" s="3" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="H10" s="3" t="s">
         <v>17</v>
@@ -1397,7 +1399,7 @@
         <v>20</v>
       </c>
       <c r="G11" s="3" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="H11" s="3" t="s">
         <v>18</v>
@@ -1435,7 +1437,7 @@
         <v>20</v>
       </c>
       <c r="G12" s="3" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="H12" s="3" t="s">
         <v>18</v>
@@ -1473,7 +1475,7 @@
         <v>20</v>
       </c>
       <c r="G13" s="3" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="H13" s="3" t="s">
         <v>18</v>
@@ -1587,7 +1589,7 @@
         <v>20</v>
       </c>
       <c r="G16" s="3" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="H16" s="3" t="s">
         <v>18</v>
@@ -1622,7 +1624,7 @@
         <v>20</v>
       </c>
       <c r="G17" s="3" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="H17" s="3" t="s">
         <v>18</v>
@@ -1701,7 +1703,7 @@
         <v>20</v>
       </c>
       <c r="G19" s="3" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="H19" s="3" t="s">
         <v>18</v>
@@ -1777,7 +1779,7 @@
         <v>20</v>
       </c>
       <c r="G21" s="3" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="H21" s="3" t="s">
         <v>18</v>
@@ -1850,7 +1852,7 @@
         <v>20</v>
       </c>
       <c r="G23" s="3" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="H23" s="3" t="s">
         <v>17</v>
@@ -1891,7 +1893,7 @@
         <v>20</v>
       </c>
       <c r="G24" s="3" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="H24" s="3" t="s">
         <v>18</v>
@@ -1938,7 +1940,7 @@
         <v>9</v>
       </c>
       <c r="L25" s="4" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="26" spans="1:13" hidden="1">
@@ -1961,7 +1963,7 @@
         <v>20</v>
       </c>
       <c r="G26" s="3" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="H26" s="3" t="s">
         <v>18</v>
@@ -1973,7 +1975,7 @@
         <v>9</v>
       </c>
       <c r="L26" s="4" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="M26" s="4" t="s">
         <v>63</v>
@@ -2014,7 +2016,7 @@
         <v>64</v>
       </c>
       <c r="M27" s="4" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="28" spans="1:13" ht="30">
@@ -2075,7 +2077,7 @@
         <v>20</v>
       </c>
       <c r="G29" s="3" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="H29" s="3" t="s">
         <v>18</v>
@@ -2093,7 +2095,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="30" spans="1:13" ht="90">
+    <row r="30" spans="1:13" ht="120">
       <c r="A30" s="3" t="s">
         <v>9</v>
       </c>
@@ -2128,7 +2130,7 @@
         <v>69</v>
       </c>
       <c r="M30" s="4" t="s">
-        <v>109</v>
+        <v>164</v>
       </c>
     </row>
     <row r="31" spans="1:13">
@@ -2186,7 +2188,7 @@
         <v>20</v>
       </c>
       <c r="G32" s="3" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="H32" s="3" t="s">
         <v>18</v>
@@ -2224,7 +2226,7 @@
         <v>20</v>
       </c>
       <c r="G33" s="3" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="H33" s="3" t="s">
         <v>18</v>
@@ -2259,7 +2261,7 @@
         <v>20</v>
       </c>
       <c r="G34" s="3" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="H34" s="3" t="s">
         <v>18</v>
@@ -2297,7 +2299,7 @@
         <v>20</v>
       </c>
       <c r="G35" s="3" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="H35" s="3" t="s">
         <v>18</v>
@@ -2332,7 +2334,7 @@
         <v>20</v>
       </c>
       <c r="G36" s="3" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="H36" s="3" t="s">
         <v>18</v>
@@ -2408,7 +2410,7 @@
         <v>20</v>
       </c>
       <c r="G38" s="3" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="H38" s="3" t="s">
         <v>18</v>
@@ -2446,7 +2448,7 @@
         <v>20</v>
       </c>
       <c r="G39" s="3" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="H39" s="3" t="s">
         <v>18</v>
@@ -2502,7 +2504,7 @@
         <v>83</v>
       </c>
       <c r="M40" s="4" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="41" spans="1:13" ht="30" hidden="1">
@@ -2525,7 +2527,7 @@
         <v>20</v>
       </c>
       <c r="G41" s="3" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="H41" s="3" t="s">
         <v>18</v>
@@ -2563,7 +2565,7 @@
         <v>20</v>
       </c>
       <c r="G42" s="3" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="H42" s="3" t="s">
         <v>18</v>
@@ -2598,7 +2600,7 @@
         <v>20</v>
       </c>
       <c r="G43" s="3" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="H43" s="3" t="s">
         <v>18</v>
@@ -2636,7 +2638,7 @@
         <v>20</v>
       </c>
       <c r="G44" s="3" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="H44" s="3" t="s">
         <v>18</v>
@@ -2674,7 +2676,7 @@
         <v>20</v>
       </c>
       <c r="G45" s="3" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="H45" s="3" t="s">
         <v>18</v>
@@ -2762,7 +2764,7 @@
         <v>101</v>
       </c>
       <c r="M47" s="4" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="48" spans="1:13" hidden="1">
@@ -2785,7 +2787,7 @@
         <v>20</v>
       </c>
       <c r="G48" s="3" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="H48" s="3" t="s">
         <v>18</v>
@@ -2820,7 +2822,7 @@
         <v>20</v>
       </c>
       <c r="G49" s="3" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="H49" s="3" t="s">
         <v>18</v>
@@ -2858,7 +2860,7 @@
         <v>20</v>
       </c>
       <c r="G50" s="3" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="H50" s="3" t="s">
         <v>17</v>
@@ -2899,7 +2901,7 @@
         <v>20</v>
       </c>
       <c r="G51" s="3" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="H51" s="3" t="s">
         <v>17</v>
@@ -2940,7 +2942,7 @@
         <v>20</v>
       </c>
       <c r="G52" s="3" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="H52" s="3" t="s">
         <v>18</v>
@@ -2987,7 +2989,7 @@
         <v>9</v>
       </c>
       <c r="L53" s="4" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="54" spans="1:13" ht="30" hidden="1">
@@ -3010,7 +3012,7 @@
         <v>20</v>
       </c>
       <c r="G54" s="3" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="H54" s="3" t="s">
         <v>17</v>
@@ -3025,15 +3027,15 @@
         <v>9</v>
       </c>
       <c r="L54" s="4" t="s">
+        <v>114</v>
+      </c>
+      <c r="M54" s="4" t="s">
         <v>115</v>
-      </c>
-      <c r="M54" s="4" t="s">
-        <v>116</v>
       </c>
     </row>
     <row r="55" spans="1:13">
       <c r="A55" s="3" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B55" s="7">
         <v>41677</v>
@@ -3063,15 +3065,15 @@
         <v>9</v>
       </c>
       <c r="L55" s="4" t="s">
+        <v>118</v>
+      </c>
+      <c r="M55" s="4" t="s">
         <v>119</v>
-      </c>
-      <c r="M55" s="4" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="56" spans="1:13">
       <c r="A56" s="3" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B56" s="7">
         <v>41677</v>
@@ -3101,12 +3103,12 @@
         <v>9</v>
       </c>
       <c r="L56" s="4" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="57" spans="1:13" ht="30" hidden="1">
       <c r="A57" s="3" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B57" s="7">
         <v>41677</v>
@@ -3124,7 +3126,7 @@
         <v>20</v>
       </c>
       <c r="G57" s="3" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="H57" s="3" t="s">
         <v>18</v>
@@ -3136,15 +3138,15 @@
         <v>9</v>
       </c>
       <c r="L57" s="4" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="M57" s="4" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="58" spans="1:13">
       <c r="A58" s="3" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B58" s="7">
         <v>41677</v>
@@ -3174,12 +3176,12 @@
         <v>9</v>
       </c>
       <c r="L58" s="4" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="59" spans="1:13">
       <c r="A59" s="3" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B59" s="7">
         <v>41677</v>
@@ -3209,7 +3211,7 @@
         <v>9</v>
       </c>
       <c r="L59" s="4" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="60" spans="1:13" hidden="1">
@@ -3232,7 +3234,7 @@
         <v>20</v>
       </c>
       <c r="G60" s="3" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="H60" s="3" t="s">
         <v>18</v>
@@ -3244,12 +3246,12 @@
         <v>9</v>
       </c>
       <c r="L60" s="4" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="61" spans="1:13" hidden="1">
       <c r="A61" s="3" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B61" s="7">
         <v>41687</v>
@@ -3267,7 +3269,7 @@
         <v>20</v>
       </c>
       <c r="G61" s="3" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="H61" s="3" t="s">
         <v>18</v>
@@ -3279,7 +3281,7 @@
         <v>9</v>
       </c>
       <c r="L61" s="4" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="62" spans="1:13" hidden="1">
@@ -3314,7 +3316,7 @@
         <v>9</v>
       </c>
       <c r="L62" s="4" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="63" spans="1:13">
@@ -3349,7 +3351,7 @@
         <v>9</v>
       </c>
       <c r="L63" s="4" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="64" spans="1:13" hidden="1">
@@ -3372,7 +3374,7 @@
         <v>20</v>
       </c>
       <c r="G64" s="3" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="H64" s="3" t="s">
         <v>18</v>
@@ -3384,7 +3386,7 @@
         <v>9</v>
       </c>
       <c r="L64" s="4" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="65" spans="1:13" hidden="1">
@@ -3407,7 +3409,7 @@
         <v>20</v>
       </c>
       <c r="G65" s="3" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="H65" s="3" t="s">
         <v>18</v>
@@ -3419,7 +3421,7 @@
         <v>9</v>
       </c>
       <c r="L65" s="4" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="66" spans="1:13" hidden="1">
@@ -3442,7 +3444,7 @@
         <v>20</v>
       </c>
       <c r="G66" s="3" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="H66" s="3" t="s">
         <v>18</v>
@@ -3454,7 +3456,7 @@
         <v>9</v>
       </c>
       <c r="L66" s="4" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="67" spans="1:13" hidden="1">
@@ -3477,7 +3479,7 @@
         <v>20</v>
       </c>
       <c r="G67" s="3" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="H67" s="3" t="s">
         <v>18</v>
@@ -3489,7 +3491,7 @@
         <v>9</v>
       </c>
       <c r="L67" s="4" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="68" spans="1:13" hidden="1">
@@ -3524,7 +3526,7 @@
         <v>9</v>
       </c>
       <c r="L68" s="4" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="69" spans="1:13" hidden="1">
@@ -3559,10 +3561,10 @@
         <v>9</v>
       </c>
       <c r="L69" s="4" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="M69" s="4" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="70" spans="1:13" ht="30" hidden="1">
@@ -3597,10 +3599,10 @@
         <v>9</v>
       </c>
       <c r="L70" s="4" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="M70" s="4" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="71" spans="1:13" ht="135">
@@ -3635,10 +3637,10 @@
         <v>9</v>
       </c>
       <c r="L71" s="4" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="M71" s="4" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="72" spans="1:13" hidden="1">
@@ -3661,7 +3663,7 @@
         <v>20</v>
       </c>
       <c r="G72" s="3" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="H72" s="3" t="s">
         <v>18</v>
@@ -3673,7 +3675,7 @@
         <v>9</v>
       </c>
       <c r="L72" s="4" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="73" spans="1:13" hidden="1">
@@ -3696,7 +3698,7 @@
         <v>20</v>
       </c>
       <c r="G73" s="3" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="H73" s="3" t="s">
         <v>18</v>
@@ -3708,7 +3710,7 @@
         <v>9</v>
       </c>
       <c r="L73" s="4" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="74" spans="1:13" hidden="1">
@@ -3731,7 +3733,7 @@
         <v>20</v>
       </c>
       <c r="G74" s="3" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="H74" s="3" t="s">
         <v>18</v>
@@ -3743,7 +3745,7 @@
         <v>9</v>
       </c>
       <c r="L74" s="4" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="75" spans="1:13" hidden="1">
@@ -3766,7 +3768,7 @@
         <v>20</v>
       </c>
       <c r="G75" s="3" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="H75" s="3" t="s">
         <v>18</v>
@@ -3778,7 +3780,7 @@
         <v>9</v>
       </c>
       <c r="L75" s="4" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="76" spans="1:13" ht="75" hidden="1">
@@ -3801,7 +3803,7 @@
         <v>20</v>
       </c>
       <c r="G76" s="3" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="H76" s="3" t="s">
         <v>17</v>
@@ -3813,15 +3815,15 @@
         <v>9</v>
       </c>
       <c r="L76" s="4" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="M76" s="4" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="77" spans="1:13" ht="30">
+      <c r="A77" s="3" t="s">
         <v>150</v>
-      </c>
-    </row>
-    <row r="77" spans="1:13">
-      <c r="A77" s="3" t="s">
-        <v>151</v>
       </c>
       <c r="B77" s="7">
         <v>41752</v>
@@ -3851,10 +3853,10 @@
         <v>9</v>
       </c>
       <c r="L77" s="4" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="M77" s="4" t="s">
-        <v>153</v>
+        <v>163</v>
       </c>
     </row>
     <row r="78" spans="1:13" hidden="1">
@@ -3877,7 +3879,7 @@
         <v>20</v>
       </c>
       <c r="G78" s="3" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="H78" s="3" t="s">
         <v>18</v>
@@ -3889,7 +3891,7 @@
         <v>9</v>
       </c>
       <c r="L78" s="4" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
     </row>
     <row r="79" spans="1:13">
@@ -3924,7 +3926,7 @@
         <v>9</v>
       </c>
       <c r="L79" s="4" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
     </row>
     <row r="80" spans="1:13" ht="30">
@@ -3941,13 +3943,13 @@
         <v>1</v>
       </c>
       <c r="E80" s="3" t="s">
-        <v>40</v>
+        <v>11</v>
       </c>
       <c r="F80" s="3" t="s">
         <v>41</v>
       </c>
       <c r="G80" s="3" t="s">
-        <v>135</v>
+        <v>35</v>
       </c>
       <c r="H80" s="3" t="s">
         <v>18</v>
@@ -3959,10 +3961,10 @@
         <v>9</v>
       </c>
       <c r="L80" s="4" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="M80" s="4" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
     </row>
     <row r="81" spans="1:13" hidden="1">
@@ -3985,7 +3987,7 @@
         <v>20</v>
       </c>
       <c r="G81" s="3" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="H81" s="3" t="s">
         <v>18</v>
@@ -3997,18 +3999,18 @@
         <v>9</v>
       </c>
       <c r="L81" s="4" t="s">
+        <v>158</v>
+      </c>
+      <c r="M81" s="4" t="s">
         <v>161</v>
       </c>
-      <c r="M81" s="4" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="82" spans="1:13" ht="30">
+    </row>
+    <row r="82" spans="1:13" ht="30" hidden="1">
       <c r="A82" s="3" t="s">
         <v>9</v>
       </c>
       <c r="B82" s="7">
-        <v>41787</v>
+        <v>41788</v>
       </c>
       <c r="C82" s="3">
         <v>1</v>
@@ -4017,140 +4019,105 @@
         <v>1</v>
       </c>
       <c r="E82" s="3" t="s">
-        <v>11</v>
+        <v>40</v>
       </c>
       <c r="F82" s="3" t="s">
-        <v>41</v>
+        <v>20</v>
       </c>
       <c r="G82" s="3" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="H82" s="3" t="s">
         <v>18</v>
       </c>
       <c r="J82" s="7">
-        <v>41787</v>
+        <v>41808</v>
       </c>
       <c r="K82" s="3" t="s">
         <v>9</v>
       </c>
       <c r="L82" s="4" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="83" spans="1:13" ht="30">
+        <v>157</v>
+      </c>
+      <c r="M82" s="4" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="83" spans="1:13" hidden="1">
       <c r="A83" s="3" t="s">
         <v>9</v>
       </c>
       <c r="B83" s="7">
-        <v>41788</v>
+        <v>41802</v>
       </c>
       <c r="C83" s="3">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="D83" s="3">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="E83" s="3" t="s">
         <v>40</v>
       </c>
       <c r="F83" s="3" t="s">
-        <v>41</v>
+        <v>20</v>
       </c>
       <c r="G83" s="3" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="H83" s="3" t="s">
         <v>18</v>
       </c>
       <c r="J83" s="7">
-        <v>41788</v>
+        <v>41802</v>
       </c>
       <c r="K83" s="3" t="s">
         <v>9</v>
       </c>
       <c r="L83" s="4" t="s">
+        <v>159</v>
+      </c>
+      <c r="M83" s="4" t="s">
         <v>160</v>
       </c>
-      <c r="M83" s="4" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="84" spans="1:13">
+    </row>
+    <row r="84" spans="1:13" hidden="1">
       <c r="A84" s="3" t="s">
         <v>9</v>
       </c>
       <c r="B84" s="7">
-        <v>41788</v>
+        <v>41808</v>
       </c>
       <c r="C84" s="3">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D84" s="3">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E84" s="3" t="s">
-        <v>11</v>
+        <v>40</v>
       </c>
       <c r="F84" s="3" t="s">
-        <v>41</v>
+        <v>20</v>
       </c>
       <c r="G84" s="3" t="s">
-        <v>158</v>
+        <v>134</v>
       </c>
       <c r="H84" s="3" t="s">
         <v>18</v>
       </c>
       <c r="J84" s="7">
-        <v>41788</v>
+        <v>41808</v>
       </c>
       <c r="K84" s="3" t="s">
         <v>9</v>
       </c>
       <c r="L84" s="4" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="85" spans="1:13" hidden="1">
-      <c r="A85" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="B85" s="7">
-        <v>41802</v>
-      </c>
-      <c r="C85" s="3">
-        <v>4</v>
-      </c>
-      <c r="D85" s="3">
-        <v>4</v>
-      </c>
-      <c r="E85" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="F85" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="G85" s="3" t="s">
-        <v>158</v>
-      </c>
-      <c r="H85" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="J85" s="7">
-        <v>41802</v>
-      </c>
-      <c r="K85" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="L85" s="4" t="s">
-        <v>163</v>
-      </c>
-      <c r="M85" s="4" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="E1:I85">
+  <autoFilter ref="E1:I84">
     <filterColumn colId="1">
       <filters>
         <filter val="New"/>

</xml_diff>

<commit_message>
Log files now have plan name in name
</commit_message>
<xml_diff>
--- a/docs/pdtoolgui_bug_list.xlsx
+++ b/docs/pdtoolgui_bug_list.xlsx
@@ -4,13 +4,13 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24709"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="32620" windowHeight="16060" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="32620" windowHeight="18720" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$E$1:$I$84</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$E$1:$I$83</definedName>
   </definedNames>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="653" uniqueCount="166">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="646" uniqueCount="165">
   <si>
     <t>Reported By</t>
   </si>
@@ -506,9 +506,6 @@
   </si>
   <si>
     <t>VCS module generator needs to have vcs connection entry in target module XML file</t>
-  </si>
-  <si>
-    <t>Plan editor for v2 of VCS module methods needs select list for VCS connection ID</t>
   </si>
   <si>
     <t>Plan editor for v2 of VCS module methods needs password field for vcsPassword argument.</t>
@@ -1000,11 +997,11 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr filterMode="1" enableFormatConditionsCalculation="0"/>
-  <dimension ref="A1:M84"/>
+  <dimension ref="A1:M83"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A40" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A85" sqref="A85"/>
+      <pane ySplit="1" topLeftCell="A30" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="K58" sqref="K58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -2130,7 +2127,7 @@
         <v>69</v>
       </c>
       <c r="M30" s="4" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="31" spans="1:13">
@@ -3161,16 +3158,16 @@
         <v>11</v>
       </c>
       <c r="F58" s="3" t="s">
-        <v>41</v>
+        <v>20</v>
       </c>
       <c r="G58" s="3" t="s">
-        <v>35</v>
+        <v>155</v>
       </c>
       <c r="H58" s="3" t="s">
         <v>18</v>
       </c>
       <c r="J58" s="7">
-        <v>41677</v>
+        <v>41808</v>
       </c>
       <c r="K58" s="3" t="s">
         <v>9</v>
@@ -3856,7 +3853,7 @@
         <v>151</v>
       </c>
       <c r="M77" s="4" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="78" spans="1:13" hidden="1">
@@ -3894,7 +3891,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="79" spans="1:13">
+    <row r="79" spans="1:13" ht="30">
       <c r="A79" s="3" t="s">
         <v>9</v>
       </c>
@@ -3902,10 +3899,10 @@
         <v>41753</v>
       </c>
       <c r="C79" s="3">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D79" s="3">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E79" s="3" t="s">
         <v>11</v>
@@ -3928,13 +3925,16 @@
       <c r="L79" s="4" t="s">
         <v>153</v>
       </c>
-    </row>
-    <row r="80" spans="1:13" ht="30">
+      <c r="M79" s="4" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="80" spans="1:13" hidden="1">
       <c r="A80" s="3" t="s">
         <v>9</v>
       </c>
       <c r="B80" s="7">
-        <v>41753</v>
+        <v>41787</v>
       </c>
       <c r="C80" s="3">
         <v>1</v>
@@ -3943,36 +3943,36 @@
         <v>1</v>
       </c>
       <c r="E80" s="3" t="s">
-        <v>11</v>
+        <v>40</v>
       </c>
       <c r="F80" s="3" t="s">
-        <v>41</v>
+        <v>20</v>
       </c>
       <c r="G80" s="3" t="s">
-        <v>35</v>
+        <v>155</v>
       </c>
       <c r="H80" s="3" t="s">
         <v>18</v>
       </c>
       <c r="J80" s="7">
-        <v>41753</v>
+        <v>41802</v>
       </c>
       <c r="K80" s="3" t="s">
         <v>9</v>
       </c>
       <c r="L80" s="4" t="s">
-        <v>154</v>
+        <v>157</v>
       </c>
       <c r="M80" s="4" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="81" spans="1:13" hidden="1">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="81" spans="1:13" ht="30" hidden="1">
       <c r="A81" s="3" t="s">
         <v>9</v>
       </c>
       <c r="B81" s="7">
-        <v>41787</v>
+        <v>41788</v>
       </c>
       <c r="C81" s="3">
         <v>1</v>
@@ -3987,36 +3987,36 @@
         <v>20</v>
       </c>
       <c r="G81" s="3" t="s">
+        <v>155</v>
+      </c>
+      <c r="H81" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="J81" s="7">
+        <v>41808</v>
+      </c>
+      <c r="K81" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="L81" s="4" t="s">
         <v>156</v>
-      </c>
-      <c r="H81" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="J81" s="7">
-        <v>41802</v>
-      </c>
-      <c r="K81" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="L81" s="4" t="s">
-        <v>158</v>
       </c>
       <c r="M81" s="4" t="s">
         <v>161</v>
       </c>
     </row>
-    <row r="82" spans="1:13" ht="30" hidden="1">
+    <row r="82" spans="1:13" hidden="1">
       <c r="A82" s="3" t="s">
         <v>9</v>
       </c>
       <c r="B82" s="7">
-        <v>41788</v>
+        <v>41802</v>
       </c>
       <c r="C82" s="3">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="D82" s="3">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="E82" s="3" t="s">
         <v>40</v>
@@ -4025,22 +4025,22 @@
         <v>20</v>
       </c>
       <c r="G82" s="3" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="H82" s="3" t="s">
         <v>18</v>
       </c>
       <c r="J82" s="7">
-        <v>41808</v>
+        <v>41802</v>
       </c>
       <c r="K82" s="3" t="s">
         <v>9</v>
       </c>
       <c r="L82" s="4" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="M82" s="4" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
     </row>
     <row r="83" spans="1:13" hidden="1">
@@ -4048,13 +4048,13 @@
         <v>9</v>
       </c>
       <c r="B83" s="7">
-        <v>41802</v>
+        <v>41808</v>
       </c>
       <c r="C83" s="3">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D83" s="3">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E83" s="3" t="s">
         <v>40</v>
@@ -4063,61 +4063,23 @@
         <v>20</v>
       </c>
       <c r="G83" s="3" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="H83" s="3" t="s">
         <v>18</v>
       </c>
       <c r="J83" s="7">
-        <v>41802</v>
+        <v>41808</v>
       </c>
       <c r="K83" s="3" t="s">
         <v>9</v>
       </c>
       <c r="L83" s="4" t="s">
-        <v>159</v>
-      </c>
-      <c r="M83" s="4" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="84" spans="1:13" hidden="1">
-      <c r="A84" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="B84" s="7">
-        <v>41808</v>
-      </c>
-      <c r="C84" s="3">
-        <v>3</v>
-      </c>
-      <c r="D84" s="3">
-        <v>3</v>
-      </c>
-      <c r="E84" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="F84" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="G84" s="3" t="s">
-        <v>134</v>
-      </c>
-      <c r="H84" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="J84" s="7">
-        <v>41808</v>
-      </c>
-      <c r="K84" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="L84" s="4" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="E1:I84">
+  <autoFilter ref="E1:I83">
     <filterColumn colId="1">
       <filters>
         <filter val="New"/>

</xml_diff>

<commit_message>
Updated for B2 release
</commit_message>
<xml_diff>
--- a/docs/pdtoolgui_bug_list.xlsx
+++ b/docs/pdtoolgui_bug_list.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24709"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24816"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="32620" windowHeight="18720" tabRatio="500"/>
+    <workbookView xWindow="5640" yWindow="720" windowWidth="32620" windowHeight="18720" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$E$1:$I$84</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$E$1:$I$87</definedName>
   </definedNames>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="661" uniqueCount="168">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="675" uniqueCount="170">
   <si>
     <t>Reported By</t>
   </si>
@@ -553,6 +553,12 @@
   </si>
   <si>
     <t>Need GUI server to call Admin API SOAP service such as getLicenses. Not trivial.</t>
+  </si>
+  <si>
+    <t>Apply updates for PDTool releases 5/28, 6/13, and 6/30</t>
+  </si>
+  <si>
+    <t>Execution plan editor shouldn't have default "server" parameter. Not all methods (vcs init) don't have server as a parameter and shouldn't output one.</t>
   </si>
 </sst>
 </file>
@@ -1006,11 +1012,11 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr filterMode="1" enableFormatConditionsCalculation="0"/>
-  <dimension ref="A1:M85"/>
+  <dimension ref="A1:M87"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A31" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A86" sqref="A86"/>
+      <pane ySplit="1" topLeftCell="A30" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A88" sqref="A88"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -4090,7 +4096,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="84" spans="1:13">
+    <row r="84" spans="1:13" hidden="1">
       <c r="A84" s="3" t="s">
         <v>9</v>
       </c>
@@ -4107,7 +4113,7 @@
         <v>40</v>
       </c>
       <c r="F84" s="3" t="s">
-        <v>41</v>
+        <v>20</v>
       </c>
       <c r="G84" s="3" t="s">
         <v>155</v>
@@ -4125,7 +4131,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="85" spans="1:13">
+    <row r="85" spans="1:13" hidden="1">
       <c r="A85" s="3" t="s">
         <v>9</v>
       </c>
@@ -4142,7 +4148,7 @@
         <v>11</v>
       </c>
       <c r="F85" s="3" t="s">
-        <v>41</v>
+        <v>20</v>
       </c>
       <c r="G85" s="3" t="s">
         <v>155</v>
@@ -4160,8 +4166,78 @@
         <v>165</v>
       </c>
     </row>
+    <row r="86" spans="1:13">
+      <c r="A86" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B86" s="7">
+        <v>41822</v>
+      </c>
+      <c r="C86" s="3">
+        <v>1</v>
+      </c>
+      <c r="D86" s="3">
+        <v>1</v>
+      </c>
+      <c r="E86" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F86" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="G86" s="3" t="s">
+        <v>155</v>
+      </c>
+      <c r="H86" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="J86" s="7">
+        <v>41822</v>
+      </c>
+      <c r="K86" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="L86" s="4" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="87" spans="1:13" ht="30" hidden="1">
+      <c r="A87" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B87" s="7">
+        <v>41841</v>
+      </c>
+      <c r="C87" s="3">
+        <v>1</v>
+      </c>
+      <c r="D87" s="3">
+        <v>1</v>
+      </c>
+      <c r="E87" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="F87" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="G87" s="3" t="s">
+        <v>155</v>
+      </c>
+      <c r="H87" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="J87" s="7">
+        <v>41841</v>
+      </c>
+      <c r="K87" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="L87" s="4" t="s">
+        <v>169</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="E1:I84">
+  <autoFilter ref="E1:I87">
     <filterColumn colId="1">
       <filters>
         <filter val="New"/>

</xml_diff>

<commit_message>
Fixed issue with writing logs during VCS init
There’s no plan during a VCS init so the plan path is null. When
ExecutePDTool was trying to generate a log file name based on the base
name of the plan path, an NPE was being thrown.
</commit_message>
<xml_diff>
--- a/docs/pdtoolgui_bug_list.xlsx
+++ b/docs/pdtoolgui_bug_list.xlsx
@@ -10,7 +10,7 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$E$1:$I$93</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$E$1:$I$94</definedName>
   </definedNames>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="720" uniqueCount="180">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="728" uniqueCount="183">
   <si>
     <t>Reported By</t>
   </si>
@@ -590,6 +590,15 @@
   <si>
     <t>Only an issue with edited deployment profile files.
 Implemented workaround of writing to temp file and copying results to deployment profile file. Not happy with it, but it works for now.</t>
+  </si>
+  <si>
+    <t>b4</t>
+  </si>
+  <si>
+    <t>ExecutePDTool class throws NPE during VCS initialization</t>
+  </si>
+  <si>
+    <t>Plan path not set. Setting plan name to "vcsinit" when plan path is null.</t>
   </si>
 </sst>
 </file>
@@ -1044,11 +1053,11 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr filterMode="1" enableFormatConditionsCalculation="0"/>
-  <dimension ref="A1:M93"/>
+  <dimension ref="A1:M94"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A28" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="M93" sqref="M93"/>
+      <pane ySplit="1" topLeftCell="A40" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A95" sqref="A95"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -4487,8 +4496,46 @@
         <v>177</v>
       </c>
     </row>
+    <row r="94" spans="1:13" ht="30" hidden="1">
+      <c r="A94" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B94" s="7">
+        <v>41880</v>
+      </c>
+      <c r="C94" s="3">
+        <v>2</v>
+      </c>
+      <c r="D94" s="3">
+        <v>2</v>
+      </c>
+      <c r="E94" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="F94" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="G94" s="3" t="s">
+        <v>180</v>
+      </c>
+      <c r="H94" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="J94" s="7">
+        <v>41880</v>
+      </c>
+      <c r="K94" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="L94" s="4" t="s">
+        <v>181</v>
+      </c>
+      <c r="M94" s="4" t="s">
+        <v>182</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="E1:I93">
+  <autoFilter ref="E1:I94">
     <filterColumn colId="1">
       <filters>
         <filter val="New"/>

</xml_diff>